<commit_message>
Add transaction confirmation in excel file
</commit_message>
<xml_diff>
--- a/RobotReaderForIDs/Output.xlsx
+++ b/RobotReaderForIDs/Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\UiPath\RoboticEnterpriseFramework\RobotReaderForIDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD435D9-1102-499B-B257-B4C451FFCF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A13407-673B-44D2-9330-E4A6215B96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1 A1 A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Modify projects and add gitignore
</commit_message>
<xml_diff>
--- a/RobotReaderForIDs/Output.xlsx
+++ b/RobotReaderForIDs/Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Documents\UiPath\RoboticEnterpriseFramework\RobotReaderForIDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A13407-673B-44D2-9330-E4A6215B96FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AC0EF6-5E4B-41C4-95EC-3CCE6CA7DD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="44">
   <si>
     <t>1790513400158</t>
   </si>
@@ -38,6 +38,15 @@
     <t>VITALIE</t>
   </si>
   <si>
+    <t>1840323114558</t>
+  </si>
+  <si>
+    <t>NEDELCU</t>
+  </si>
+  <si>
+    <t>EMIL</t>
+  </si>
+  <si>
     <t>1891128125803</t>
   </si>
   <si>
@@ -47,100 +56,109 @@
     <t>BOGDAN</t>
   </si>
   <si>
+    <t>1891113341181</t>
+  </si>
+  <si>
+    <t>ISPILANTE</t>
+  </si>
+  <si>
+    <t>SENTIMENT BRUSLI</t>
+  </si>
+  <si>
+    <t>1460913400088</t>
+  </si>
+  <si>
+    <t>POPESCU</t>
+  </si>
+  <si>
+    <t>MARIN</t>
+  </si>
+  <si>
+    <t>1740416350016</t>
+  </si>
+  <si>
+    <t>ERDOGAN</t>
+  </si>
+  <si>
+    <t>MURAD-ALIN</t>
+  </si>
+  <si>
+    <t>1781017431536</t>
+  </si>
+  <si>
+    <t>BRIA</t>
+  </si>
+  <si>
+    <t>ALEXANDRU-BOGDAN</t>
+  </si>
+  <si>
+    <t>22800202237896</t>
+  </si>
+  <si>
+    <t>MIREA</t>
+  </si>
+  <si>
+    <t>VICTORIA-VERONICA</t>
+  </si>
+  <si>
+    <t>1511104131251</t>
+  </si>
+  <si>
+    <t>BASESCU</t>
+  </si>
+  <si>
+    <t>TRAIAN</t>
+  </si>
+  <si>
+    <t>ȘIEVCIUK</t>
+  </si>
+  <si>
+    <t>EUJEN</t>
+  </si>
+  <si>
+    <t>1531028197506</t>
+  </si>
+  <si>
+    <t>GATES</t>
+  </si>
+  <si>
+    <t>BILL</t>
+  </si>
+  <si>
+    <t>1430413126190</t>
+  </si>
+  <si>
+    <t>BARA</t>
+  </si>
+  <si>
+    <t>IOSIF</t>
+  </si>
+  <si>
+    <t>1950218114549</t>
+  </si>
+  <si>
+    <t>MILULESCU</t>
+  </si>
+  <si>
+    <t>IOAN</t>
+  </si>
+  <si>
     <t>46091340008</t>
   </si>
   <si>
-    <t>POPESCU</t>
-  </si>
-  <si>
-    <t>MARIN</t>
-  </si>
-  <si>
     <t>178101743153</t>
   </si>
   <si>
-    <t>BRIA</t>
-  </si>
-  <si>
     <t>ALEXANDRU-BO G D A N</t>
   </si>
   <si>
-    <t>1511104131251</t>
-  </si>
-  <si>
-    <t>BASESCU</t>
-  </si>
-  <si>
-    <t>TRAIAN</t>
-  </si>
-  <si>
-    <t>1531028197506</t>
-  </si>
-  <si>
-    <t>GATES</t>
-  </si>
-  <si>
-    <t>BILL</t>
-  </si>
-  <si>
-    <t>1950218114549</t>
-  </si>
-  <si>
-    <t>MILULESCU</t>
-  </si>
-  <si>
-    <t>IOAN</t>
-  </si>
-  <si>
-    <t>1840323114558</t>
-  </si>
-  <si>
-    <t>NEDELCU</t>
-  </si>
-  <si>
-    <t>EMIL</t>
-  </si>
-  <si>
-    <t>1891113341181</t>
-  </si>
-  <si>
-    <t>ISPILANTE</t>
-  </si>
-  <si>
-    <t>SENTIMENT BRUSLI</t>
-  </si>
-  <si>
-    <t>1740416350016</t>
-  </si>
-  <si>
-    <t>ERDOGAN</t>
-  </si>
-  <si>
-    <t>MURAD-ALIN</t>
-  </si>
-  <si>
     <t>NP22800202237896</t>
   </si>
   <si>
-    <t>MIREA</t>
-  </si>
-  <si>
-    <t>VICTORIA-VERONICA</t>
-  </si>
-  <si>
-    <t>ȘIEVCIUK</t>
-  </si>
-  <si>
-    <t>EUJEN</t>
-  </si>
-  <si>
-    <t>1430413126190</t>
-  </si>
-  <si>
-    <t>BARA</t>
-  </si>
-  <si>
-    <t>IOSIF</t>
+    <t>CNP already exist</t>
+  </si>
+  <si>
+    <t>Successful</t>
   </si>
 </sst>
 </file>
@@ -507,20 +525,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1 C1 C1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,8 +549,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -541,8 +563,11 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -553,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -564,7 +589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -575,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -586,7 +611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -597,7 +622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -608,7 +633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -619,31 +644,31 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>33</v>
@@ -652,7 +677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -670,7 +695,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1 A1 A1:C1"/>
@@ -691,133 +716,276 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>